<commit_message>
Moved excel file into Foster_care
</commit_message>
<xml_diff>
--- a/Qualitative_research/Foster_Care/Research-Foster_care.xlsx
+++ b/Qualitative_research/Foster_Care/Research-Foster_care.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/Qualitative_research/Foster_Care/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E67BDFF7-70FB-4C43-B2F0-349F3D145EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD58780-D3AD-2C44-8648-703C0BA6DD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{7863E363-D8A0-424A-9594-405E1C7C063E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="55">
   <si>
     <t>ID</t>
   </si>
@@ -52,6 +52,153 @@
   </si>
   <si>
     <t>Program</t>
+  </si>
+  <si>
+    <t>Loudoun</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Foster Care</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great Expectations </t>
+  </si>
+  <si>
+    <t>Education and Training Voucher (ETV) Program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Independent Living Program </t>
+  </si>
+  <si>
+    <t>Practical Nursing Program</t>
+  </si>
+  <si>
+    <t>Adult High School</t>
+  </si>
+  <si>
+    <t>English Learners (EL) - Aprenda Ingles</t>
+  </si>
+  <si>
+    <t>GED Prep School</t>
+  </si>
+  <si>
+    <t>Adult Education Catalog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employment </t>
+  </si>
+  <si>
+    <t>Workforce Innovation and Opportunity Act</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additonal courses that can be taken at Loudoun County Public Schools; prices range from $50 - $200 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offers preparatory classes provides basic skills instruction to adults whose math and reading skills have been assessed at or below the GED® readiness level; Each session = $180 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given in reading, writing, listening, and speaking;    Classes meet twice a week - 13 week; $170 total </t>
+  </si>
+  <si>
+    <t xml:space="preserve">18+; Designed for individuals who need between one (1) and ten (10) credits to complete their Standard High School Diploma requirements; $300 per course </t>
+  </si>
+  <si>
+    <t xml:space="preserve">18+; 2-year program; total cost : $6,100; Must take TEAS exam prior </t>
+  </si>
+  <si>
+    <t>ages 14-21; assists in developing the skills necessary to make the transition from foster care to independent living; Department of Social Services; Age out = 21</t>
+  </si>
+  <si>
+    <t>14 - 25 years of age who either aged out of foster care or still in fsoter care; Funds can be applied toward, but not limited to, colleges, universities, community colleges, vocational programs, and one-year training institution</t>
+  </si>
+  <si>
+    <t>17-24 year olds affiliated with the Virginia Foster Care System; Connecting them to community resources, scholarship opportunities and other support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18-24; Department of Labor; 1-on-1 training, resume building, interview prep, labor market review, etc. ; need verification of foster care or receiving public assistance </t>
+  </si>
+  <si>
+    <t>Northern Virginia Educating Youth through Employment (EYE)</t>
+  </si>
+  <si>
+    <t>18-24; Summer initiative that recruits, screens and matches youth  with professional opportunities in the private sector and other area businesses</t>
+  </si>
+  <si>
+    <t>Loudoun Workforce Resource Center Community Partners</t>
+  </si>
+  <si>
+    <t>lists all of the county's partners that can help young adults find employment, housing, educational opportunities, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Housing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transportation </t>
+  </si>
+  <si>
+    <t>Route 54 (Safe T-ride)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loudoun County Local Bus Service; Free for all in the county; Runs every 20 mins at 10 stops </t>
+  </si>
+  <si>
+    <t>Medicaid Transportation (LogistiCare)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Must have Medicaid number; non-emergency and urgent medical appointments; Must make requests 5 days early; Department of Medical Assistance Services </t>
+  </si>
+  <si>
+    <t>On Demand Transportation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Department of Family Services; Must fall below 70% of State Median Income; make requests 5 days prior; Locally, to UVA and Georgetown Hospital </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insurances </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Funding &amp; Policy </t>
+  </si>
+  <si>
+    <t>Family Access to Medical Insurance Security Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">covers all the medical care that growing children need to stay healthy and if they get sick or hurt; no enrollment costs or monthly premiums; no copays; under 19 years old, not insured and fall below family income of $2,201 monthly </t>
+  </si>
+  <si>
+    <t>Virginia Medicaid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ages 18 to 26 can get Medicaid if they were in foster care and had Medicaid in any state on their 18th birthday; no income limit for former foster care youths </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allegheny </t>
+  </si>
+  <si>
+    <t>Continuum of Care (CoC)</t>
+  </si>
+  <si>
+    <t>US Department of Housing and Urban Development; Awarded vouchers to provide stable housing for young adults (18-24) who have aged out of the foster care system</t>
+  </si>
+  <si>
+    <t>SkillSource Group Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serves as fiscal agent and entity that pursues additional funding sources for the board of Workforce Innovation and Opportunity Training and Employment programs </t>
+  </si>
+  <si>
+    <t>Educational and Training Vouchers (ETVs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virginia Department of Social Services through the federal government; Provides  financial assistance of up to $5,000 per year for up to five years for college, career school, or training </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assists community college students in Virginia with financial need; this is funded by the state or federal </t>
+  </si>
+  <si>
+    <t>Community College Tuition Grants</t>
   </si>
 </sst>
 </file>
@@ -94,9 +241,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,15 +564,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C922EE-0460-9E4F-801F-98245821615D}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="C20" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="34" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="34.5" style="3" customWidth="1"/>
+    <col min="6" max="6" width="46" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -435,11 +591,582 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <f>A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f t="shared" ref="A5:A27" si="0">A4+1</f>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <f t="shared" ref="A28:A35" si="1">A27+1</f>
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added JaiDa's programs to excel sheet
</commit_message>
<xml_diff>
--- a/Qualitative_research/Foster_Care/Research-Foster_care.xlsx
+++ b/Qualitative_research/Foster_Care/Research-Foster_care.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/Qualitative_research/Foster_Care/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C64E0D7-1A8B-294E-AB4E-38D8A1C5669A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53A9C0E-8234-3643-8410-2A7124182672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{7863E363-D8A0-424A-9594-405E1C7C063E}"/>
   </bookViews>
@@ -579,7 +579,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B10" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>